<commit_message>
casi terminamos las temporizaciones
</commit_message>
<xml_diff>
--- a/Matrices/TInvariantes.xlsx
+++ b/Matrices/TInvariantes.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -380,11 +380,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>